<commit_message>
2019-11-27 +Update: Use Case +Update: AP Description +Update: Risk Map
+Update: Use Case: Added the last use case description (searching for track).
+Update: AP Description: Added AP description from Core Layer.
+Update: Risk Map: Added one risk and changed the risk code to generate a risk map out of it.
</commit_message>
<xml_diff>
--- a/doc/2019_PM_Tabellen_PMH.xlsx
+++ b/doc/2019_PM_Tabellen_PMH.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hagenberg\ESD - FH OOE Hagenberg\1 Semester\ISE1-Uebung\Virtuelle Jukebox Share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Dropbox\Hagenberg\ESD - FH OOE Hagenberg\1 Semester\ISE1-Uebung\Jukebox-App\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066403A9-B0AE-4E31-8E84-A41EE162A189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personaleinsatzplan" sheetId="4" r:id="rId1"/>
     <sheet name="Personalkosten" sheetId="5" r:id="rId2"/>
     <sheet name="Projektkosten" sheetId="3" r:id="rId3"/>
+    <sheet name="Risk Map" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Personaleinsatzplan!$A:$B,Personaleinsatzplan!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Personalkosten!#REF!,Personalkosten!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="66">
   <si>
     <t>PSP-Code</t>
   </si>
@@ -208,12 +208,36 @@
   </si>
   <si>
     <t>Nunner</t>
+  </si>
+  <si>
+    <t>R000</t>
+  </si>
+  <si>
+    <t>R001</t>
+  </si>
+  <si>
+    <t>R002</t>
+  </si>
+  <si>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>Linie</t>
+  </si>
+  <si>
+    <t>R004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -735,7 +759,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="1">
       <tableStyleElement type="wholeTable" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -755,6 +779,1401 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Risk</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Map</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Risk Map'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>R000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>R001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>R002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>R003</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{32D88274-BAE5-4F4B-A950-0831ED1D13D1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-9130-4AE9-B6BF-B8B16DA080D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{86774D94-F46B-4FE0-A76F-6EEAF745C70A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-9130-4AE9-B6BF-B8B16DA080D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{12D28C60-2819-43C5-BFEE-E97D6F309838}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-9130-4AE9-B6BF-B8B16DA080D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BC7A7B05-824F-495F-A91A-0CF8450BAF63}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-9130-4AE9-B6BF-B8B16DA080D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risk Map'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Risk Map'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Risk Map'!$A$2:$A$5</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>R000</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>R001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>R002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>R003</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9130-4AE9-B6BF-B8B16DA080D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2102849328"/>
+        <c:axId val="2102849744"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>break line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risk Map'!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Risk Map'!$G$2:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9130-4AE9-B6BF-B8B16DA080D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="178813456"/>
+        <c:axId val="2102853488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2102849328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Eintrittswahrscheinlichkeit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> / [%]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2102849744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2102849744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1600"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Risikokosten</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> / [€]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2102849328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2102853488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1600"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="178813456"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="178813456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2102853488"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,23 +2252,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -885,23 +2287,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1077,23 +2462,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="3.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.8984375" style="1" customWidth="1"/>
+    <col min="3" max="7" width="3.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.8984375" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="66.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="66.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +2504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +2522,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>28</v>
       </c>
@@ -1165,7 +2550,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>29</v>
       </c>
@@ -1192,7 +2577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>30</v>
       </c>
@@ -1219,7 +2604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>31</v>
       </c>
@@ -1246,7 +2631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +2648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +2675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
@@ -1317,7 +2702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +2729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
@@ -1371,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -1398,7 +2783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
         <v>3</v>
       </c>
@@ -1415,7 +2800,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>32</v>
       </c>
@@ -1442,7 +2827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>33</v>
       </c>
@@ -1469,7 +2854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
@@ -1496,7 +2881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>35</v>
       </c>
@@ -1523,7 +2908,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>4</v>
       </c>
@@ -1540,7 +2925,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>36</v>
       </c>
@@ -1567,7 +2952,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1595,7 +2980,7 @@
       </c>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1622,7 +3007,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>39</v>
       </c>
@@ -1649,7 +3034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>48</v>
       </c>
@@ -1676,13 +3061,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H24" s="30">
         <f>H2+H7+H13+H18</f>
         <v>192.5</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:15" ht="11" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -1693,23 +3078,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.69921875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="5.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="5.7109375" style="1"/>
+    <col min="1" max="1" width="7.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.8984375" style="1" customWidth="1"/>
+    <col min="3" max="7" width="5.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.69921875" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="5.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="50.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +3120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
       <c r="B2" s="44" t="s">
         <v>54</v>
@@ -1757,7 +3142,7 @@
       </c>
       <c r="H2" s="42"/>
     </row>
-    <row r="3" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
@@ -1775,7 +3160,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
@@ -1808,7 +3193,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>29</v>
       </c>
@@ -1840,7 +3225,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>30</v>
       </c>
@@ -1872,7 +3257,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>31</v>
       </c>
@@ -1904,7 +3289,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>6</v>
       </c>
@@ -1921,7 +3306,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>7</v>
       </c>
@@ -1953,7 +3338,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -1985,7 +3370,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
@@ -2017,7 +3402,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>43</v>
       </c>
@@ -2049,7 +3434,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>44</v>
       </c>
@@ -2081,7 +3466,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36">
         <v>3</v>
       </c>
@@ -2098,7 +3483,7 @@
         <v>7350</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
@@ -2130,7 +3515,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>33</v>
       </c>
@@ -2162,7 +3547,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
@@ -2194,7 +3579,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>35</v>
       </c>
@@ -2226,7 +3611,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>4</v>
       </c>
@@ -2243,7 +3628,7 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>36</v>
       </c>
@@ -2275,7 +3660,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>37</v>
       </c>
@@ -2307,7 +3692,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>38</v>
       </c>
@@ -2339,7 +3724,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>39</v>
       </c>
@@ -2371,7 +3756,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>48</v>
       </c>
@@ -2403,13 +3788,13 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="11.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="40">
         <f>H19+H14+H8+H3</f>
         <v>19250</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:8" ht="11" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -2420,21 +3805,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.59765625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="6.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.09765625" style="1" customWidth="1"/>
+    <col min="3" max="7" width="6.69921875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="81.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="81.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +3842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -2485,7 +3870,7 @@
         <v>4350</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>28</v>
       </c>
@@ -2504,7 +3889,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>29</v>
       </c>
@@ -2523,7 +3908,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>30</v>
       </c>
@@ -2542,7 +3927,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>31</v>
       </c>
@@ -2561,7 +3946,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -2589,7 +3974,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
@@ -2608,7 +3993,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
@@ -2624,7 +4009,7 @@
       <c r="F9" s="52"/>
       <c r="G9" s="53"/>
     </row>
-    <row r="10" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
@@ -2640,7 +4025,7 @@
       <c r="F10" s="52"/>
       <c r="G10" s="53"/>
     </row>
-    <row r="11" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
@@ -2659,7 +4044,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -2678,7 +4063,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36">
         <v>3</v>
       </c>
@@ -2706,7 +4091,7 @@
         <v>7350</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>32</v>
       </c>
@@ -2725,7 +4110,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>33</v>
       </c>
@@ -2744,7 +4129,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
@@ -2763,7 +4148,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>35</v>
       </c>
@@ -2782,7 +4167,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="36">
         <v>4</v>
       </c>
@@ -2810,7 +4195,7 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>36</v>
       </c>
@@ -2829,7 +4214,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>37</v>
       </c>
@@ -2848,7 +4233,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>38</v>
       </c>
@@ -2867,7 +4252,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>39</v>
       </c>
@@ -2886,7 +4271,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>48</v>
       </c>
@@ -2905,15 +4290,103 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G24" s="51">
         <f>G18+G13+G7+G2</f>
         <v>19250</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>